<commit_message>
update high roll starter codes
</commit_message>
<xml_diff>
--- a/spring20/assignment02/Grading Template - assignment02.xlsx
+++ b/spring20/assignment02/Grading Template - assignment02.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aavol\Documents\LMU\CMSI 186 - Spring 2020\Github\Volosin\cmsi186\spring20\assignment02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6288EB8C-2FF0-4777-8E50-58ADA6B6BE9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC00038A-CAE5-4E78-99B8-FBEF12672E50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" xr2:uid="{4D734FBB-B9F3-4B7F-B685-E161468322F2}"/>
   </bookViews>
@@ -192,19 +192,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,9 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C3E5AC-318A-4CE9-B6C3-BA51F4BF3A12}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="155" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -543,219 +544,219 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="8"/>
+      <c r="B13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="9" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
-      <c r="B20" s="9" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
-      <c r="B21" s="9" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-      <c r="B22" s="9" t="s">
+      <c r="A22" s="7"/>
+      <c r="B22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C26">

</xml_diff>